<commit_message>
rubric update for today's work
</commit_message>
<xml_diff>
--- a/Project Rubric (062020).xlsx
+++ b/Project Rubric (062020).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585F3595-5129-4513-92EA-DE351DF0F87D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE6149-5AFA-463D-98AE-79FA87D8D97F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -611,10 +611,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -940,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,11 +1075,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1148,7 +1144,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 16, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 16,0)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 16, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 16,0)</f>
@@ -1228,7 +1224,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 16, IF(H10+I4 &gt; 16, 16- I4, H10),0)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 16, IF(I10+J4 &gt; 16, 16- J4, I10),0)</f>
@@ -1297,7 +1293,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 16 &gt; 0, K4+H4 - 16, 0)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 16 &gt; 0, H10+I4 - 16, 0)</f>
@@ -1710,11 +1706,15 @@
       <c r="D28" s="24">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2154,7 +2154,9 @@
       <c r="D46" s="24">
         <v>1</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="16">
         <f t="shared" si="0"/>

</xml_diff>